<commit_message>
250124 IDEA pom relation deal
</commit_message>
<xml_diff>
--- a/EasyExcel-private/src/main/resources/template/company_import.xlsx
+++ b/EasyExcel-private/src/main/resources/template/company_import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9420"/>
+    <workbookView windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="入驻企业" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">入驻企业!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -259,13 +272,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -284,34 +297,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -325,14 +310,6 @@
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -377,6 +354,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -422,7 +414,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -456,49 +469,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -510,121 +607,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -647,21 +660,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -694,6 +692,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -752,148 +765,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -904,64 +917,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1235,12 +1248,12 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7962962962963" defaultRowHeight="24" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="32.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="20.3333333333333" customWidth="1"/>
     <col min="2" max="2" width="15.8888888888889" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.1111111111111" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.1111111111111" customWidth="1"/>
@@ -1249,7 +1262,7 @@
     <col min="7" max="7" width="26.1111111111111" customWidth="1"/>
     <col min="8" max="8" width="16.1111111111111" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.1111111111111" customWidth="1"/>
-    <col min="10" max="10" width="28.7777777777778" customWidth="1"/>
+    <col min="10" max="10" width="15.4444444444444" customWidth="1"/>
     <col min="11" max="11" width="35.5555555555556" customWidth="1"/>
     <col min="12" max="12" width="31.4444444444444" customWidth="1"/>
   </cols>
@@ -1295,23 +1308,23 @@
   </sheetData>
   <sheetProtection formatCells="0" insertHyperlinks="0" autoFilter="0"/>
   <dataValidations count="7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:D1 F1:G1"/>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="错误提示" error="请输入下拉列表中的一个值" sqref="B2:B1048576">
       <formula1>"50人以下,50-100人,100-150人,500-1000人,1000人以上"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 D1 F1 G1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1>"稀土产业,网络安全产业,再生铝产业,充电桩产业,氢能产业,钴产业,机器人产业,工业软件产业,游戏产业,光伏产业,锂电产业,化工产业,电子产业,储能产业,led产业,云计算产业,新材料产业,服装产业,铜产业,pcb产业,医美产业,文具产业,风电产业,人工智能产业"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>"农林牧渔,建筑建材,冶金矿产,石油化工,水利水电,交通运输,信息产业,机械机电,轻工食品,服装纺织,专业服务,安全防护,环保绿化,旅游休闲,电子电工,办公文教,玩具礼品,家居用品,物资,包装,体育,办公,生物医疗"</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="输入内容有误" error="请输入正确的日期" sqref="H2:H1048576">
-      <formula1>1</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>"稀土产业,网络安全产业,再生铝产业,充电桩产业,氢能产业,钴产业,机器人产业,工业软件产业,游戏产业,光伏产业,锂电产业,化工产业,电子产业,储能产业,led产业,云计算产业,新材料产业,服装产业,铜产业,pcb产业,医美产业,文具产业,风电产业,人工智能产业"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="错误提示" error="请输入下拉列表中的一个值" sqref="E2:E1048576">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576 G2:G1048576">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="输入内容有误" error="请输入正确的日期" sqref="H2:H1048576">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G1048576">
       <formula1>"是,否"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>